<commit_message>
changes in kholodenko example code
</commit_message>
<xml_diff>
--- a/PyCoTools/Examples/KholodenkoExample/fitItemTemplate.xlsx
+++ b/PyCoTools/Examples/KholodenkoExample/fitItemTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="1764"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>StartValue</t>
   </si>
@@ -37,54 +37,21 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>(phosphorylation of MAPKK).KK3</t>
-  </si>
-  <si>
-    <t>(MAPKKK activation).K1</t>
-  </si>
-  <si>
     <t>(dephosphorylation of MAPK-PP).V9</t>
   </si>
   <si>
-    <t>(phosphorylation of MAPK-P).k8</t>
-  </si>
-  <si>
-    <t>(MAPKKK inactivation).KK2</t>
-  </si>
-  <si>
-    <t>(MAPKKK inactivation).V2</t>
-  </si>
-  <si>
-    <t>(phosphorylation of MAPKK-P).k4</t>
-  </si>
-  <si>
-    <t>(dephosphorylation of MAPKK-PP).KK5</t>
-  </si>
-  <si>
     <t>(dephosphorylation of MAPK-PP).KK9</t>
   </si>
   <si>
     <t>(dephosphorylation of MAPKK-P).KK6</t>
   </si>
   <si>
-    <t>(phosphorylation of MAPKK-P).KK4</t>
-  </si>
-  <si>
-    <t>(MAPKKK activation).V1</t>
-  </si>
-  <si>
-    <t>(MAPKKK activation).Ki</t>
-  </si>
-  <si>
     <t>(phosphorylation of MAPK).KK7</t>
   </si>
   <si>
     <t>(dephosphorylation of MAPK-P).KK10</t>
   </si>
   <si>
-    <t>(phosphorylation of MAPK-P).KK8</t>
-  </si>
-  <si>
     <t>(dephosphorylation of MAPK-P).V10</t>
   </si>
   <si>
@@ -94,33 +61,12 @@
     <t>15</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>0.5</t>
   </si>
   <si>
-    <t>0.025</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>0.75</t>
   </si>
   <si>
-    <t>1e-06</t>
-  </si>
-  <si>
     <t>1000000</t>
   </si>
   <si>
@@ -130,52 +76,19 @@
     <t>ReactionParameter</t>
   </si>
   <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPKK],ParameterGroup=Parameters,Parameter=KK3</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=K1</t>
-  </si>
-  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-PP],ParameterGroup=Parameters,Parameter=V9</t>
   </si>
   <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=k8</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK inactivation],ParameterGroup=Parameters,Parameter=KK2</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK inactivation],ParameterGroup=Parameters,Parameter=V2</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPKK-P],ParameterGroup=Parameters,Parameter=k4</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPKK-PP],ParameterGroup=Parameters,Parameter=KK5</t>
-  </si>
-  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-PP],ParameterGroup=Parameters,Parameter=KK9</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPKK-P],ParameterGroup=Parameters,Parameter=KK6</t>
   </si>
   <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPKK-P],ParameterGroup=Parameters,Parameter=KK4</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=V1</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=Ki</t>
-  </si>
-  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPK],ParameterGroup=Parameters,Parameter=KK7</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=KK10</t>
-  </si>
-  <si>
-    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=KK8</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=V10</t>
@@ -547,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,416 +502,163 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D3">
-        <v>10000</v>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
+      <c r="C4" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6">
-        <v>0.1</v>
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
+      <c r="C7" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
+        <v>14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="D10" s="2">
-        <v>100</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>10000</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2">
-        <v>10000</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="D13" s="2">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14">
-        <v>100</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>100</v>
-      </c>
-      <c r="E15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2">
-        <v>10</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1000</v>
-      </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>100000</v>
-      </c>
-      <c r="E19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1006,5 +666,6 @@
     <sortCondition ref="A15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed 'DotSize' to 'MarkerSize' in pycopi.TimeCourse for consistancy
</commit_message>
<xml_diff>
--- a/PyCoTools/Examples/KholodenkoExample/fitItemTemplate.xlsx
+++ b/PyCoTools/Examples/KholodenkoExample/fitItemTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="1764"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
   <si>
     <t>StartValue</t>
   </si>
@@ -37,34 +37,121 @@
     <t>Parameter</t>
   </si>
   <si>
+    <t>(phosphorylation of MAPKK).KK3</t>
+  </si>
+  <si>
+    <t>(MAPKKK activation).K1</t>
+  </si>
+  <si>
     <t>(dephosphorylation of MAPK-PP).V9</t>
   </si>
   <si>
+    <t>(phosphorylation of MAPK).k7</t>
+  </si>
+  <si>
+    <t>(phosphorylation of MAPK-P).k8</t>
+  </si>
+  <si>
+    <t>(MAPKKK inactivation).KK2</t>
+  </si>
+  <si>
+    <t>(MAPKKK inactivation).V2</t>
+  </si>
+  <si>
+    <t>(phosphorylation of MAPKK-P).k4</t>
+  </si>
+  <si>
+    <t>(dephosphorylation of MAPKK-PP).KK5</t>
+  </si>
+  <si>
     <t>(dephosphorylation of MAPK-PP).KK9</t>
   </si>
   <si>
     <t>(dephosphorylation of MAPKK-P).KK6</t>
   </si>
   <si>
+    <t>(phosphorylation of MAPKK-P).KK4</t>
+  </si>
+  <si>
+    <t>(MAPKKK activation).Ki</t>
+  </si>
+  <si>
     <t>(phosphorylation of MAPK).KK7</t>
   </si>
   <si>
     <t>(dephosphorylation of MAPK-P).KK10</t>
   </si>
   <si>
+    <t>(phosphorylation of MAPK-P).KK8</t>
+  </si>
+  <si>
     <t>(dephosphorylation of MAPK-P).V10</t>
   </si>
   <si>
     <t>(dephosphorylation of MAPKK-P).V6</t>
   </si>
   <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.75</t>
+    <t>(MAPKKK activation).n</t>
+  </si>
+  <si>
+    <t>11.3054</t>
+  </si>
+  <si>
+    <t>1.18045</t>
+  </si>
+  <si>
+    <t>0.00871167</t>
+  </si>
+  <si>
+    <t>0.0191301</t>
+  </si>
+  <si>
+    <t>0.155267</t>
+  </si>
+  <si>
+    <t>228.991</t>
+  </si>
+  <si>
+    <t>1.35247</t>
+  </si>
+  <si>
+    <t>0.0571224</t>
+  </si>
+  <si>
+    <t>0.0325145</t>
+  </si>
+  <si>
+    <t>2749.2</t>
+  </si>
+  <si>
+    <t>3407.78</t>
+  </si>
+  <si>
+    <t>77.4387</t>
+  </si>
+  <si>
+    <t>5.27274</t>
+  </si>
+  <si>
+    <t>0.00161673</t>
+  </si>
+  <si>
+    <t>63.1385</t>
+  </si>
+  <si>
+    <t>530.369</t>
+  </si>
+  <si>
+    <t>0.0198492</t>
+  </si>
+  <si>
+    <t>41.3158</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>1e-06</t>
   </si>
   <si>
     <t>1000000</t>
@@ -76,25 +163,61 @@
     <t>ReactionParameter</t>
   </si>
   <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPKK],ParameterGroup=Parameters,Parameter=KK3</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=K1</t>
+  </si>
+  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-PP],ParameterGroup=Parameters,Parameter=V9</t>
   </si>
   <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPK],ParameterGroup=Parameters,Parameter=k7</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=k8</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK inactivation],ParameterGroup=Parameters,Parameter=KK2</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK inactivation],ParameterGroup=Parameters,Parameter=V2</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPKK-P],ParameterGroup=Parameters,Parameter=k4</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPKK-PP],ParameterGroup=Parameters,Parameter=KK5</t>
+  </si>
+  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-PP],ParameterGroup=Parameters,Parameter=KK9</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPKK-P],ParameterGroup=Parameters,Parameter=KK6</t>
   </si>
   <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPKK-P],ParameterGroup=Parameters,Parameter=KK4</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=Ki</t>
+  </si>
+  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPK],ParameterGroup=Parameters,Parameter=KK7</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=KK10</t>
   </si>
   <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[phosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=KK8</t>
+  </si>
+  <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPK-P],ParameterGroup=Parameters,Parameter=V10</t>
   </si>
   <si>
     <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[dephosphorylation of MAPKK-P],ParameterGroup=Parameters,Parameter=V6</t>
+  </si>
+  <si>
+    <t>CN=Root,Model=Kholodenko2000 - Ultrasensitivity and negative feedback bring oscillations in MAPK cascade,Vector=Reactions[MAPKKK activation],ParameterGroup=Parameters,Parameter=n</t>
   </si>
 </sst>
 </file>
@@ -153,12 +276,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,21 +582,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="173.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -502,170 +618,445 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2">
-        <v>9.9999999999999995E-7</v>
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>23</v>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G22">
-    <sortCondition ref="A15"/>
+  <sortState ref="A2:G23">
+    <sortCondition ref="A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started adding multi process to Run
</commit_message>
<xml_diff>
--- a/PyCoTools/Examples/KholodenkoExample/fitItemTemplate.xlsx
+++ b/PyCoTools/Examples/KholodenkoExample/fitItemTemplate.xlsx
@@ -585,12 +585,18 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="173.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>